<commit_message>
final stage of V2 [3]
</commit_message>
<xml_diff>
--- a/TestTraffic.xlsx
+++ b/TestTraffic.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>E1</t>
   </si>
@@ -406,43 +406,13 @@
     <t>Karaj</t>
   </si>
   <si>
-    <t>Kerman</t>
-  </si>
-  <si>
-    <t>Bandar Abbas</t>
-  </si>
-  <si>
-    <t>Rasht</t>
-  </si>
-  <si>
-    <t>Arak</t>
-  </si>
-  <si>
-    <t>Restored</t>
-  </si>
-  <si>
     <t>Tehran</t>
   </si>
   <si>
-    <t>Mashhad</t>
-  </si>
-  <si>
-    <t>Esfahan</t>
-  </si>
-  <si>
-    <t>Shiraz</t>
-  </si>
-  <si>
-    <t>Ahwaz</t>
-  </si>
-  <si>
-    <t>Tabriz</t>
-  </si>
-  <si>
-    <t>Babol</t>
-  </si>
-  <si>
-    <t>Hamedan</t>
+    <t>Qom</t>
+  </si>
+  <si>
+    <t>Damavand</t>
   </si>
 </sst>
 </file>
@@ -1042,34 +1012,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1358,11 +1328,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AO14" sqref="AO14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="42" max="42" width="3.77734375" customWidth="1"/>
+    <col min="43" max="45" width="8.88671875" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:85" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
@@ -1374,68 +1348,68 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="51" t="s">
+      <c r="K1" s="47"/>
+      <c r="L1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="50"/>
-      <c r="N1" s="51" t="s">
+      <c r="M1" s="47"/>
+      <c r="N1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="49" t="s">
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="49" t="s">
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="49" t="s">
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="44" t="s">
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="49" t="s">
         <v>6</v>
       </c>
       <c r="AD1" s="45"/>
       <c r="AE1" s="45"/>
       <c r="AF1" s="45"/>
       <c r="AG1" s="45"/>
-      <c r="AH1" s="52" t="s">
+      <c r="AH1" s="50" t="s">
         <v>7</v>
       </c>
       <c r="AI1" s="45"/>
       <c r="AJ1" s="45"/>
       <c r="AK1" s="45"/>
-      <c r="AL1" s="52" t="s">
+      <c r="AL1" s="50" t="s">
         <v>8</v>
       </c>
       <c r="AM1" s="45"/>
       <c r="AN1" s="45"/>
       <c r="AO1" s="45"/>
-      <c r="AP1" s="52" t="s">
+      <c r="AP1" s="50" t="s">
         <v>9</v>
       </c>
       <c r="AQ1" s="45"/>
       <c r="AR1" s="45"/>
       <c r="AS1" s="45"/>
-      <c r="AT1" s="52" t="s">
+      <c r="AT1" s="50" t="s">
         <v>10</v>
       </c>
       <c r="AU1" s="45"/>
       <c r="AV1" s="45"/>
-      <c r="AW1" s="53"/>
+      <c r="AW1" s="51"/>
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="AZ1" s="4"/>
@@ -1443,47 +1417,47 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="5"/>
-      <c r="BE1" s="48" t="s">
+      <c r="BE1" s="44" t="s">
         <v>11</v>
       </c>
       <c r="BF1" s="45"/>
       <c r="BG1" s="45"/>
-      <c r="BH1" s="44" t="s">
+      <c r="BH1" s="49" t="s">
         <v>12</v>
       </c>
       <c r="BI1" s="45"/>
       <c r="BJ1" s="45"/>
-      <c r="BK1" s="44" t="s">
+      <c r="BK1" s="49" t="s">
         <v>13</v>
       </c>
       <c r="BL1" s="45"/>
       <c r="BM1" s="45"/>
-      <c r="BN1" s="44" t="s">
+      <c r="BN1" s="49" t="s">
         <v>14</v>
       </c>
       <c r="BO1" s="45"/>
       <c r="BP1" s="45"/>
-      <c r="BQ1" s="46" t="s">
+      <c r="BQ1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
+      <c r="BR1" s="52"/>
+      <c r="BS1" s="52"/>
+      <c r="BT1" s="52"/>
+      <c r="BU1" s="52"/>
+      <c r="BV1" s="52"/>
+      <c r="BW1" s="52"/>
+      <c r="BX1" s="52"/>
       <c r="BY1" s="6"/>
-      <c r="BZ1" s="47" t="s">
+      <c r="BZ1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="CA1" s="47"/>
-      <c r="CB1" s="47"/>
-      <c r="CC1" s="47"/>
-      <c r="CD1" s="47"/>
-      <c r="CE1" s="47"/>
-      <c r="CF1" s="47"/>
-      <c r="CG1" s="47"/>
+      <c r="CA1" s="53"/>
+      <c r="CB1" s="53"/>
+      <c r="CC1" s="53"/>
+      <c r="CD1" s="53"/>
+      <c r="CE1" s="53"/>
+      <c r="CF1" s="53"/>
+      <c r="CG1" s="53"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
@@ -1745,10 +1719,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -1773,7 +1747,9 @@
       <c r="V3" s="17"/>
       <c r="W3" s="17"/>
       <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
+      <c r="Y3" s="17">
+        <v>7</v>
+      </c>
       <c r="Z3" s="17"/>
       <c r="AA3" s="17"/>
       <c r="AB3" s="17"/>
@@ -1787,7 +1763,7 @@
       <c r="AJ3" s="21"/>
       <c r="AK3" s="21"/>
       <c r="AL3" s="20">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="AM3" s="21"/>
       <c r="AN3" s="21"/>
@@ -1850,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
@@ -1878,7 +1854,9 @@
       <c r="V4" s="28"/>
       <c r="W4" s="28"/>
       <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
+      <c r="Y4" s="28">
+        <v>2</v>
+      </c>
       <c r="Z4" s="28"/>
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
@@ -1892,7 +1870,7 @@
       <c r="AJ4" s="31"/>
       <c r="AK4" s="31"/>
       <c r="AL4" s="30">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="AM4" s="31"/>
       <c r="AN4" s="31"/>
@@ -1955,10 +1933,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="29"/>
@@ -1983,7 +1961,9 @@
       <c r="V5" s="28"/>
       <c r="W5" s="28"/>
       <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
+      <c r="Y5" s="28">
+        <v>7</v>
+      </c>
       <c r="Z5" s="28"/>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
@@ -1997,7 +1977,7 @@
       <c r="AJ5" s="31"/>
       <c r="AK5" s="31"/>
       <c r="AL5" s="30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AM5" s="31"/>
       <c r="AN5" s="31"/>
@@ -2007,7 +1987,7 @@
       <c r="AR5" s="31"/>
       <c r="AS5" s="31"/>
       <c r="AT5" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU5" s="33">
         <v>100</v>
@@ -2060,10 +2040,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="29"/>
@@ -2088,7 +2068,9 @@
       <c r="V6" s="28"/>
       <c r="W6" s="28"/>
       <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
+      <c r="Y6" s="28">
+        <v>2</v>
+      </c>
       <c r="Z6" s="28"/>
       <c r="AA6" s="28"/>
       <c r="AB6" s="28"/>
@@ -2102,7 +2084,7 @@
       <c r="AJ6" s="31"/>
       <c r="AK6" s="31"/>
       <c r="AL6" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM6" s="31"/>
       <c r="AN6" s="31"/>
@@ -2160,24 +2142,22 @@
       <c r="CF6" s="28"/>
       <c r="CG6" s="34"/>
     </row>
-    <row r="7" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="29"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="41">
-        <v>1</v>
-      </c>
+      <c r="I7" s="41"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="29"/>
@@ -2206,9 +2186,7 @@
       <c r="AI7" s="31"/>
       <c r="AJ7" s="31"/>
       <c r="AK7" s="31"/>
-      <c r="AL7" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL7" s="30"/>
       <c r="AM7" s="31"/>
       <c r="AN7" s="31"/>
       <c r="AO7" s="31"/>
@@ -2217,17 +2195,11 @@
       <c r="AR7" s="31"/>
       <c r="AS7" s="31"/>
       <c r="AT7" s="32">
-        <v>2</v>
-      </c>
-      <c r="AU7" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV7" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW7" s="33" t="s">
-        <v>94</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AU7" s="33"/>
+      <c r="AV7" s="33"/>
+      <c r="AW7" s="33"/>
       <c r="AX7" s="28"/>
       <c r="AY7" s="28"/>
       <c r="AZ7" s="28"/>
@@ -2265,24 +2237,22 @@
       <c r="CF7" s="28"/>
       <c r="CG7" s="34"/>
     </row>
-    <row r="8" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
       <c r="H8" s="37"/>
-      <c r="I8" s="41">
-        <v>2</v>
-      </c>
+      <c r="I8" s="41"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
       <c r="L8" s="29"/>
@@ -2311,9 +2281,7 @@
       <c r="AI8" s="31"/>
       <c r="AJ8" s="31"/>
       <c r="AK8" s="31"/>
-      <c r="AL8" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL8" s="30"/>
       <c r="AM8" s="31"/>
       <c r="AN8" s="31"/>
       <c r="AO8" s="31"/>
@@ -2324,15 +2292,9 @@
       <c r="AT8" s="32">
         <v>1</v>
       </c>
-      <c r="AU8" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV8" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW8" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AU8" s="33"/>
+      <c r="AV8" s="33"/>
+      <c r="AW8" s="33"/>
       <c r="AX8" s="28"/>
       <c r="AY8" s="28"/>
       <c r="AZ8" s="28"/>
@@ -2370,24 +2332,16 @@
       <c r="CF8" s="28"/>
       <c r="CG8" s="34"/>
     </row>
-    <row r="9" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>7</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>106</v>
-      </c>
+    <row r="9" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="37"/>
-      <c r="I9" s="41">
-        <v>3</v>
-      </c>
+      <c r="I9" s="41"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" s="29"/>
@@ -2416,9 +2370,7 @@
       <c r="AI9" s="31"/>
       <c r="AJ9" s="31"/>
       <c r="AK9" s="31"/>
-      <c r="AL9" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL9" s="30"/>
       <c r="AM9" s="31"/>
       <c r="AN9" s="31"/>
       <c r="AO9" s="31"/>
@@ -2426,18 +2378,10 @@
       <c r="AQ9" s="31"/>
       <c r="AR9" s="31"/>
       <c r="AS9" s="31"/>
-      <c r="AT9" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU9" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV9" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW9" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT9" s="32"/>
+      <c r="AU9" s="33"/>
+      <c r="AV9" s="33"/>
+      <c r="AW9" s="33"/>
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="28"/>
@@ -2475,24 +2419,16 @@
       <c r="CF9" s="28"/>
       <c r="CG9" s="34"/>
     </row>
-    <row r="10" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>104</v>
-      </c>
+    <row r="10" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="28"/>
       <c r="E10" s="29"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
       <c r="H10" s="37"/>
-      <c r="I10" s="41">
-        <v>4</v>
-      </c>
+      <c r="I10" s="41"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
       <c r="L10" s="29"/>
@@ -2521,9 +2457,7 @@
       <c r="AI10" s="31"/>
       <c r="AJ10" s="31"/>
       <c r="AK10" s="31"/>
-      <c r="AL10" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL10" s="30"/>
       <c r="AM10" s="31"/>
       <c r="AN10" s="31"/>
       <c r="AO10" s="31"/>
@@ -2531,18 +2465,10 @@
       <c r="AQ10" s="31"/>
       <c r="AR10" s="31"/>
       <c r="AS10" s="31"/>
-      <c r="AT10" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU10" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV10" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW10" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT10" s="32"/>
+      <c r="AU10" s="33"/>
+      <c r="AV10" s="33"/>
+      <c r="AW10" s="33"/>
       <c r="AX10" s="28"/>
       <c r="AY10" s="28"/>
       <c r="AZ10" s="28"/>
@@ -2580,24 +2506,16 @@
       <c r="CF10" s="28"/>
       <c r="CG10" s="34"/>
     </row>
-    <row r="11" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>105</v>
-      </c>
+    <row r="11" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="28"/>
       <c r="E11" s="29"/>
       <c r="F11" s="28"/>
       <c r="G11" s="38"/>
       <c r="H11" s="37"/>
-      <c r="I11" s="35">
-        <v>1</v>
-      </c>
+      <c r="I11" s="35"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
       <c r="L11" s="29"/>
@@ -2626,9 +2544,7 @@
       <c r="AI11" s="31"/>
       <c r="AJ11" s="31"/>
       <c r="AK11" s="31"/>
-      <c r="AL11" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL11" s="30"/>
       <c r="AM11" s="31"/>
       <c r="AN11" s="31"/>
       <c r="AO11" s="31"/>
@@ -2636,18 +2552,10 @@
       <c r="AQ11" s="31"/>
       <c r="AR11" s="31"/>
       <c r="AS11" s="31"/>
-      <c r="AT11" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU11" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV11" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW11" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT11" s="32"/>
+      <c r="AU11" s="33"/>
+      <c r="AV11" s="33"/>
+      <c r="AW11" s="33"/>
       <c r="AX11" s="28"/>
       <c r="AY11" s="28"/>
       <c r="AZ11" s="28"/>
@@ -2685,24 +2593,16 @@
       <c r="CF11" s="28"/>
       <c r="CG11" s="34"/>
     </row>
-    <row r="12" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25">
-        <v>10</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>106</v>
-      </c>
+    <row r="12" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
       <c r="F12" s="37"/>
       <c r="G12" s="39"/>
       <c r="H12" s="40"/>
-      <c r="I12" s="35">
-        <v>2</v>
-      </c>
+      <c r="I12" s="35"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
       <c r="L12" s="29"/>
@@ -2731,9 +2631,7 @@
       <c r="AI12" s="31"/>
       <c r="AJ12" s="31"/>
       <c r="AK12" s="31"/>
-      <c r="AL12" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL12" s="30"/>
       <c r="AM12" s="31"/>
       <c r="AN12" s="31"/>
       <c r="AO12" s="31"/>
@@ -2741,18 +2639,10 @@
       <c r="AQ12" s="31"/>
       <c r="AR12" s="31"/>
       <c r="AS12" s="31"/>
-      <c r="AT12" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU12" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV12" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW12" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT12" s="32"/>
+      <c r="AU12" s="33"/>
+      <c r="AV12" s="33"/>
+      <c r="AW12" s="33"/>
       <c r="AX12" s="28"/>
       <c r="AY12" s="28"/>
       <c r="AZ12" s="28"/>
@@ -2790,24 +2680,16 @@
       <c r="CF12" s="28"/>
       <c r="CG12" s="34"/>
     </row>
-    <row r="13" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25">
-        <v>11</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>95</v>
-      </c>
+    <row r="13" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="28"/>
       <c r="E13" s="29"/>
       <c r="F13" s="28"/>
       <c r="G13" s="17"/>
       <c r="H13" s="37"/>
-      <c r="I13" s="35">
-        <v>3</v>
-      </c>
+      <c r="I13" s="35"/>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
       <c r="L13" s="29"/>
@@ -2836,9 +2718,7 @@
       <c r="AI13" s="31"/>
       <c r="AJ13" s="31"/>
       <c r="AK13" s="31"/>
-      <c r="AL13" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL13" s="30"/>
       <c r="AM13" s="31"/>
       <c r="AN13" s="31"/>
       <c r="AO13" s="31"/>
@@ -2846,18 +2726,10 @@
       <c r="AQ13" s="31"/>
       <c r="AR13" s="31"/>
       <c r="AS13" s="31"/>
-      <c r="AT13" s="32">
-        <v>2</v>
-      </c>
-      <c r="AU13" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV13" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW13" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT13" s="32"/>
+      <c r="AU13" s="33"/>
+      <c r="AV13" s="33"/>
+      <c r="AW13" s="33"/>
       <c r="AX13" s="28"/>
       <c r="AY13" s="28"/>
       <c r="AZ13" s="28"/>
@@ -2895,24 +2767,16 @@
       <c r="CF13" s="28"/>
       <c r="CG13" s="34"/>
     </row>
-    <row r="14" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25">
-        <v>12</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>107</v>
-      </c>
+    <row r="14" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="28"/>
       <c r="E14" s="29"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="37"/>
-      <c r="I14" s="35">
-        <v>4</v>
-      </c>
+      <c r="I14" s="35"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
       <c r="L14" s="29"/>
@@ -2941,9 +2805,7 @@
       <c r="AI14" s="31"/>
       <c r="AJ14" s="31"/>
       <c r="AK14" s="31"/>
-      <c r="AL14" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL14" s="30"/>
       <c r="AM14" s="31"/>
       <c r="AN14" s="31"/>
       <c r="AO14" s="31"/>
@@ -2951,18 +2813,10 @@
       <c r="AQ14" s="31"/>
       <c r="AR14" s="31"/>
       <c r="AS14" s="31"/>
-      <c r="AT14" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU14" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV14" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW14" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT14" s="32"/>
+      <c r="AU14" s="33"/>
+      <c r="AV14" s="33"/>
+      <c r="AW14" s="33"/>
       <c r="AX14" s="28"/>
       <c r="AY14" s="28"/>
       <c r="AZ14" s="28"/>
@@ -3000,24 +2854,16 @@
       <c r="CF14" s="28"/>
       <c r="CG14" s="34"/>
     </row>
-    <row r="15" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25">
-        <v>13</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>96</v>
-      </c>
+    <row r="15" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="37"/>
-      <c r="I15" s="41">
-        <v>1</v>
-      </c>
+      <c r="I15" s="41"/>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
       <c r="L15" s="29"/>
@@ -3046,9 +2892,7 @@
       <c r="AI15" s="31"/>
       <c r="AJ15" s="31"/>
       <c r="AK15" s="31"/>
-      <c r="AL15" s="30">
-        <v>22</v>
-      </c>
+      <c r="AL15" s="30"/>
       <c r="AM15" s="31"/>
       <c r="AN15" s="31"/>
       <c r="AO15" s="31"/>
@@ -3056,18 +2900,10 @@
       <c r="AQ15" s="31"/>
       <c r="AR15" s="31"/>
       <c r="AS15" s="31"/>
-      <c r="AT15" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU15" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV15" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW15" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT15" s="32"/>
+      <c r="AU15" s="33"/>
+      <c r="AV15" s="33"/>
+      <c r="AW15" s="33"/>
       <c r="AX15" s="28"/>
       <c r="AY15" s="28"/>
       <c r="AZ15" s="28"/>
@@ -3105,24 +2941,16 @@
       <c r="CF15" s="28"/>
       <c r="CG15" s="34"/>
     </row>
-    <row r="16" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="25">
-        <v>14</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>97</v>
-      </c>
+    <row r="16" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="37"/>
-      <c r="I16" s="41">
-        <v>2</v>
-      </c>
+      <c r="I16" s="41"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="29"/>
@@ -3151,9 +2979,7 @@
       <c r="AI16" s="31"/>
       <c r="AJ16" s="31"/>
       <c r="AK16" s="31"/>
-      <c r="AL16" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL16" s="30"/>
       <c r="AM16" s="31"/>
       <c r="AN16" s="31"/>
       <c r="AO16" s="31"/>
@@ -3161,18 +2987,10 @@
       <c r="AQ16" s="31"/>
       <c r="AR16" s="31"/>
       <c r="AS16" s="31"/>
-      <c r="AT16" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU16" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV16" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW16" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT16" s="32"/>
+      <c r="AU16" s="33"/>
+      <c r="AV16" s="33"/>
+      <c r="AW16" s="33"/>
       <c r="AX16" s="28"/>
       <c r="AY16" s="28"/>
       <c r="AZ16" s="28"/>
@@ -3210,24 +3028,16 @@
       <c r="CF16" s="28"/>
       <c r="CG16" s="34"/>
     </row>
-    <row r="17" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25">
-        <v>15</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>108</v>
-      </c>
+    <row r="17" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="28"/>
       <c r="E17" s="29"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="41">
-        <v>3</v>
-      </c>
+      <c r="I17" s="41"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
       <c r="L17" s="29"/>
@@ -3256,9 +3066,7 @@
       <c r="AI17" s="31"/>
       <c r="AJ17" s="31"/>
       <c r="AK17" s="31"/>
-      <c r="AL17" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL17" s="30"/>
       <c r="AM17" s="31"/>
       <c r="AN17" s="31"/>
       <c r="AO17" s="31"/>
@@ -3266,18 +3074,10 @@
       <c r="AQ17" s="31"/>
       <c r="AR17" s="31"/>
       <c r="AS17" s="31"/>
-      <c r="AT17" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU17" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV17" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW17" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT17" s="32"/>
+      <c r="AU17" s="33"/>
+      <c r="AV17" s="33"/>
+      <c r="AW17" s="33"/>
       <c r="AX17" s="28"/>
       <c r="AY17" s="28"/>
       <c r="AZ17" s="28"/>
@@ -3315,24 +3115,16 @@
       <c r="CF17" s="28"/>
       <c r="CG17" s="34"/>
     </row>
-    <row r="18" spans="1:85" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="25">
-        <v>16</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>98</v>
-      </c>
+    <row r="18" spans="1:85" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="37"/>
-      <c r="I18" s="41">
-        <v>4</v>
-      </c>
+      <c r="I18" s="41"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
       <c r="L18" s="29"/>
@@ -3361,9 +3153,7 @@
       <c r="AI18" s="31"/>
       <c r="AJ18" s="31"/>
       <c r="AK18" s="31"/>
-      <c r="AL18" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL18" s="30"/>
       <c r="AM18" s="31"/>
       <c r="AN18" s="31"/>
       <c r="AO18" s="31"/>
@@ -3371,18 +3161,10 @@
       <c r="AQ18" s="31"/>
       <c r="AR18" s="31"/>
       <c r="AS18" s="31"/>
-      <c r="AT18" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU18" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV18" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW18" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="AT18" s="32"/>
+      <c r="AU18" s="33"/>
+      <c r="AV18" s="33"/>
+      <c r="AW18" s="33"/>
       <c r="AX18" s="28"/>
       <c r="AY18" s="28"/>
       <c r="AZ18" s="28"/>
@@ -3421,23 +3203,15 @@
       <c r="CG18" s="34"/>
     </row>
     <row r="19" spans="1:85" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <v>17</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>99</v>
-      </c>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="28"/>
       <c r="E19" s="29"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="37"/>
-      <c r="I19" s="35">
-        <v>1</v>
-      </c>
+      <c r="I19" s="35"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
       <c r="L19" s="29"/>
@@ -3466,9 +3240,7 @@
       <c r="AI19" s="31"/>
       <c r="AJ19" s="31"/>
       <c r="AK19" s="31"/>
-      <c r="AL19" s="30">
-        <v>2</v>
-      </c>
+      <c r="AL19" s="30"/>
       <c r="AM19" s="31"/>
       <c r="AN19" s="31"/>
       <c r="AO19" s="31"/>
@@ -3476,18 +3248,10 @@
       <c r="AQ19" s="31"/>
       <c r="AR19" s="31"/>
       <c r="AS19" s="31"/>
-      <c r="AT19" s="32">
-        <v>1</v>
-      </c>
-      <c r="AU19" s="33">
-        <v>100</v>
-      </c>
-      <c r="AV19" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW19" s="33" t="s">
-        <v>100</v>
-      </c>
+      <c r="AT19" s="32"/>
+      <c r="AU19" s="33"/>
+      <c r="AV19" s="33"/>
+      <c r="AW19" s="33"/>
       <c r="AX19" s="28"/>
       <c r="AY19" s="28"/>
       <c r="AZ19" s="28"/>
@@ -3533,6 +3297,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BH1:BJ1"/>
+    <mergeCell ref="BK1:BM1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BQ1:BX1"/>
+    <mergeCell ref="BZ1:CG1"/>
     <mergeCell ref="BE1:BG1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -3545,11 +3314,6 @@
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="BK1:BM1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BQ1:BX1"/>
-    <mergeCell ref="BZ1:CG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
grooming and rwa algorithms added (final V2 [4])
</commit_message>
<xml_diff>
--- a/TestTraffic.xlsx
+++ b/TestTraffic.xlsx
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AK9" sqref="AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2173,7 +2173,9 @@
       <c r="V7" s="28"/>
       <c r="W7" s="28"/>
       <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
+      <c r="Y7" s="28">
+        <v>0</v>
+      </c>
       <c r="Z7" s="28"/>
       <c r="AA7" s="28"/>
       <c r="AB7" s="28"/>
@@ -2186,7 +2188,9 @@
       <c r="AI7" s="31"/>
       <c r="AJ7" s="31"/>
       <c r="AK7" s="31"/>
-      <c r="AL7" s="30"/>
+      <c r="AL7" s="30">
+        <v>0</v>
+      </c>
       <c r="AM7" s="31"/>
       <c r="AN7" s="31"/>
       <c r="AO7" s="31"/>
@@ -2268,7 +2272,9 @@
       <c r="V8" s="28"/>
       <c r="W8" s="28"/>
       <c r="X8" s="28"/>
-      <c r="Y8" s="28"/>
+      <c r="Y8" s="28">
+        <v>0</v>
+      </c>
       <c r="Z8" s="28"/>
       <c r="AA8" s="28"/>
       <c r="AB8" s="28"/>
@@ -2281,7 +2287,9 @@
       <c r="AI8" s="31"/>
       <c r="AJ8" s="31"/>
       <c r="AK8" s="31"/>
-      <c r="AL8" s="30"/>
+      <c r="AL8" s="30">
+        <v>0</v>
+      </c>
       <c r="AM8" s="31"/>
       <c r="AN8" s="31"/>
       <c r="AO8" s="31"/>

</xml_diff>

<commit_message>
enhancing demand map and bug fixing
</commit_message>
<xml_diff>
--- a/TestTraffic.xlsx
+++ b/TestTraffic.xlsx
@@ -1012,12 +1012,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1028,18 +1037,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AK9" sqref="AK9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,68 +1348,68 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="48" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="47"/>
-      <c r="N1" s="48" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="46" t="s">
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="46" t="s">
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="46" t="s">
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="47"/>
-      <c r="AA1" s="47"/>
-      <c r="AB1" s="47"/>
-      <c r="AC1" s="49" t="s">
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="44" t="s">
         <v>6</v>
       </c>
       <c r="AD1" s="45"/>
       <c r="AE1" s="45"/>
       <c r="AF1" s="45"/>
       <c r="AG1" s="45"/>
-      <c r="AH1" s="50" t="s">
+      <c r="AH1" s="52" t="s">
         <v>7</v>
       </c>
       <c r="AI1" s="45"/>
       <c r="AJ1" s="45"/>
       <c r="AK1" s="45"/>
-      <c r="AL1" s="50" t="s">
+      <c r="AL1" s="52" t="s">
         <v>8</v>
       </c>
       <c r="AM1" s="45"/>
       <c r="AN1" s="45"/>
       <c r="AO1" s="45"/>
-      <c r="AP1" s="50" t="s">
+      <c r="AP1" s="52" t="s">
         <v>9</v>
       </c>
       <c r="AQ1" s="45"/>
       <c r="AR1" s="45"/>
       <c r="AS1" s="45"/>
-      <c r="AT1" s="50" t="s">
+      <c r="AT1" s="52" t="s">
         <v>10</v>
       </c>
       <c r="AU1" s="45"/>
       <c r="AV1" s="45"/>
-      <c r="AW1" s="51"/>
+      <c r="AW1" s="53"/>
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="AZ1" s="4"/>
@@ -1417,47 +1417,47 @@
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
       <c r="BD1" s="5"/>
-      <c r="BE1" s="44" t="s">
+      <c r="BE1" s="48" t="s">
         <v>11</v>
       </c>
       <c r="BF1" s="45"/>
       <c r="BG1" s="45"/>
-      <c r="BH1" s="49" t="s">
+      <c r="BH1" s="44" t="s">
         <v>12</v>
       </c>
       <c r="BI1" s="45"/>
       <c r="BJ1" s="45"/>
-      <c r="BK1" s="49" t="s">
+      <c r="BK1" s="44" t="s">
         <v>13</v>
       </c>
       <c r="BL1" s="45"/>
       <c r="BM1" s="45"/>
-      <c r="BN1" s="49" t="s">
+      <c r="BN1" s="44" t="s">
         <v>14</v>
       </c>
       <c r="BO1" s="45"/>
       <c r="BP1" s="45"/>
-      <c r="BQ1" s="52" t="s">
+      <c r="BQ1" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="BR1" s="52"/>
-      <c r="BS1" s="52"/>
-      <c r="BT1" s="52"/>
-      <c r="BU1" s="52"/>
-      <c r="BV1" s="52"/>
-      <c r="BW1" s="52"/>
-      <c r="BX1" s="52"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
       <c r="BY1" s="6"/>
-      <c r="BZ1" s="53" t="s">
+      <c r="BZ1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="CA1" s="53"/>
-      <c r="CB1" s="53"/>
-      <c r="CC1" s="53"/>
-      <c r="CD1" s="53"/>
-      <c r="CE1" s="53"/>
-      <c r="CF1" s="53"/>
-      <c r="CG1" s="53"/>
+      <c r="CA1" s="47"/>
+      <c r="CB1" s="47"/>
+      <c r="CC1" s="47"/>
+      <c r="CD1" s="47"/>
+      <c r="CE1" s="47"/>
+      <c r="CF1" s="47"/>
+      <c r="CG1" s="47"/>
     </row>
     <row r="2" spans="1:85" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
@@ -1719,10 +1719,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="18"/>
@@ -3305,11 +3305,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BH1:BJ1"/>
-    <mergeCell ref="BK1:BM1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BQ1:BX1"/>
-    <mergeCell ref="BZ1:CG1"/>
     <mergeCell ref="BE1:BG1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
@@ -3322,6 +3317,11 @@
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="BH1:BJ1"/>
+    <mergeCell ref="BK1:BM1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BQ1:BX1"/>
+    <mergeCell ref="BZ1:CG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>